<commit_message>
Iniciando inclusao de horas
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -494,7 +494,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="26.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="29.6640625" customWidth="1" min="2" max="2"/>
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="B1" s="9" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B2" s="9" t="n">
-        <v>2021</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="3">
@@ -602,7 +602,7 @@
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -1488,7 +1488,7 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -2374,7 +2374,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -3260,7 +3260,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -4146,7 +4146,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -5032,7 +5032,7 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -5918,7 +5918,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -6804,7 +6804,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -7690,7 +7690,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -8576,7 +8576,7 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -9461,7 +9461,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -10347,7 +10347,7 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -11233,7 +11233,7 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -12120,7 +12120,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -13008,7 +13008,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -13894,7 +13894,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -14780,7 +14780,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -15666,7 +15666,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -16552,7 +16552,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.5546875" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>

</xml_diff>